<commit_message>
Added registration of secondary columns
The method _registerValueHeaderEntry register a column without header
entry to the right of an existing column, such that a value can be
retrieved with parseLine().
</commit_message>
<xml_diff>
--- a/t/testfile.xlsx
+++ b/t/testfile.xlsx
@@ -422,7 +422,7 @@
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;8Income&amp;C&amp;8&amp;R&amp;8&amp;P of &amp;N</oddHeader>
-    <oddFooter>&amp;L&amp;8Generated by Cool Tool v1.3&amp;C&amp;8Created: 2013-5-3 - 14:2:17&amp;R&amp;8Boogy Warehouses / Purchase division</oddFooter>
+    <oddFooter>&amp;L&amp;8Generated by Cool Tool v1.3&amp;C&amp;8Created: 2013-5-3 - 17:39:34&amp;R&amp;8Boogy Warehouses / Purchase division</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -449,7 +449,7 @@
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;8Balance&amp;C&amp;8&amp;R&amp;8&amp;P of &amp;N</oddHeader>
-    <oddFooter>&amp;L&amp;8Generated by Cool Tool v1.3&amp;C&amp;8Created: 2013-5-3 - 14:2:17&amp;R&amp;8Boogy Warehouses / Purchase division</oddFooter>
+    <oddFooter>&amp;L&amp;8Generated by Cool Tool v1.3&amp;C&amp;8Created: 2013-5-3 - 17:39:34&amp;R&amp;8Boogy Warehouses / Purchase division</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>